<commit_message>
Vertex Addition averages complete
</commit_message>
<xml_diff>
--- a/Data/Scenarios/Graph List and Stats.xlsx
+++ b/Data/Scenarios/Graph List and Stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marto\git\Algos_Assignment1\Data\Generated New\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marto\git\Algos_Assignment1\Data\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644B907C-C36C-45C9-9E7B-017B8CACCEA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B327F59-BDE3-49A4-BC22-760E231DE379}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24324" yWindow="228" windowWidth="21252" windowHeight="13608" activeTab="2" xr2:uid="{61CBB812-40D1-44A3-AFF3-2B0F76CA3C04}"/>
+    <workbookView xWindow="24516" yWindow="204" windowWidth="21252" windowHeight="13608" activeTab="2" xr2:uid="{61CBB812-40D1-44A3-AFF3-2B0F76CA3C04}"/>
   </bookViews>
   <sheets>
     <sheet name="AdjList" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="66">
   <si>
     <t>Filename</t>
   </si>
@@ -224,13 +224,16 @@
     <t>khop average time (50 iterations)</t>
   </si>
   <si>
-    <t>100 Additions</t>
-  </si>
-  <si>
-    <t>100 Deletions</t>
-  </si>
-  <si>
     <t>khop average time (average taken from 50 iterations)</t>
+  </si>
+  <si>
+    <t>Vertex Additions</t>
+  </si>
+  <si>
+    <t>Vertex Deletions</t>
+  </si>
+  <si>
+    <t>adding 10,000 vertices (avg. of total 5 iterations)</t>
   </si>
 </sst>
 </file>
@@ -594,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D71CDE3-7DBD-462C-93FC-85AE65D9340E}">
   <dimension ref="B1:L57"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,15 +607,17 @@
     <col min="3" max="3" width="13.88671875" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -637,10 +642,10 @@
         <v>60</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
@@ -661,6 +666,9 @@
       </c>
       <c r="H3" s="2">
         <v>4.6680257999999898E-4</v>
+      </c>
+      <c r="K3">
+        <v>4.1898774E-3</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
@@ -682,6 +690,9 @@
       <c r="H4" s="2">
         <v>5.3750067999999999E-4</v>
       </c>
+      <c r="K4">
+        <v>4.2035464E-3</v>
+      </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -702,6 +713,9 @@
       <c r="H5" s="2">
         <v>6.7331398000000002E-4</v>
       </c>
+      <c r="K5">
+        <v>4.2000909999999995E-3</v>
+      </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -722,6 +736,9 @@
       <c r="H6">
         <v>3.912428448E-2</v>
       </c>
+      <c r="K6">
+        <v>4.1613680000000004E-3</v>
+      </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -742,6 +759,9 @@
       <c r="H7">
         <v>4.0837181179999897E-2</v>
       </c>
+      <c r="K7">
+        <v>4.0930466000000006E-3</v>
+      </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
@@ -762,6 +782,9 @@
       <c r="H8">
         <v>4.536798014E-2</v>
       </c>
+      <c r="K8">
+        <v>4.1389820000000003E-3</v>
+      </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
@@ -781,6 +804,9 @@
       </c>
       <c r="H9">
         <v>0.29823591620000001</v>
+      </c>
+      <c r="K9">
+        <v>4.0835239999999998E-3</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -802,6 +828,9 @@
       <c r="H10">
         <v>0.34319052485999901</v>
       </c>
+      <c r="K10">
+        <v>4.3289534000000001E-3</v>
+      </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
@@ -822,6 +851,9 @@
       <c r="H11">
         <v>0.29742041835999999</v>
       </c>
+      <c r="K11">
+        <v>4.1073207999999996E-3</v>
+      </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -842,6 +874,9 @@
       <c r="H12">
         <v>5.2149841379999999E-2</v>
       </c>
+      <c r="K12">
+        <v>5.5171611999999997E-3</v>
+      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
@@ -862,6 +897,9 @@
       <c r="H13">
         <v>2.3810141140000001E-2</v>
       </c>
+      <c r="K13">
+        <v>5.5179883999999998E-3</v>
+      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -882,6 +920,9 @@
       <c r="H14">
         <v>2.2179341419999998E-2</v>
       </c>
+      <c r="K14">
+        <v>5.5127730000000003E-3</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
@@ -902,6 +943,9 @@
       <c r="H15">
         <v>2.3086100533199998</v>
       </c>
+      <c r="K15">
+        <v>5.4580388000000004E-3</v>
+      </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -922,8 +966,11 @@
       <c r="H16">
         <v>3.0831228558400001</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>5.1006119999999992E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -942,8 +989,11 @@
       <c r="H17">
         <v>6.2140992448799999</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <v>5.5419514E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -962,8 +1012,11 @@
       <c r="H18">
         <v>32.387339088860003</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>5.2144037999999997E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -982,8 +1035,11 @@
       <c r="H19">
         <v>28.8205005797799</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>5.1482734000000002E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -1002,8 +1058,11 @@
       <c r="H20">
         <v>17.050284592560001</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>5.5584432000000007E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>20</v>
       </c>
@@ -1022,8 +1081,11 @@
       <c r="H21">
         <v>5.8952841199999897E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>3.9834663999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -1042,8 +1104,11 @@
       <c r="H22">
         <v>5.7988563819999901E-2</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K22">
+        <v>3.9325925999999997E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -1062,8 +1127,11 @@
       <c r="H23">
         <v>3.4127632319999997E-2</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K23">
+        <v>3.9686584E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -1082,8 +1150,11 @@
       <c r="H24">
         <v>11.3893343637</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K24">
+        <v>3.8832249999999997E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -1102,8 +1173,11 @@
       <c r="H25">
         <v>8.6356112273600001</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K25">
+        <v>4.3103598000000009E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>25</v>
       </c>
@@ -1113,8 +1187,11 @@
       <c r="D26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>4.0892934000000001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -1124,8 +1201,11 @@
       <c r="D27">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>4.2214573999999998E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -1135,8 +1215,11 @@
       <c r="D28">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K28">
+        <v>3.9811339999999999E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -1146,8 +1229,11 @@
       <c r="D29">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K29">
+        <v>4.1286610000000005E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -1166,8 +1252,11 @@
       <c r="H31" s="2">
         <v>3.7747419999999998E-5</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K31">
+        <v>4.2718132000000002E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -1186,8 +1275,11 @@
       <c r="H32" s="2">
         <v>4.1874739999999997E-5</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K32">
+        <v>4.1670347999999994E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -1206,8 +1298,11 @@
       <c r="H33" s="2">
         <v>4.8186219999999998E-5</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K33">
+        <v>4.1079228000000002E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -1226,8 +1321,11 @@
       <c r="H34">
         <v>4.8287935200000002E-3</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K34">
+        <v>4.484073600000001E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -1246,8 +1344,11 @@
       <c r="H35">
         <v>4.9460617199999996E-3</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K35">
+        <v>4.1477922E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -1266,8 +1367,11 @@
       <c r="H36">
         <v>5.3350818400000003E-3</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K36">
+        <v>4.0735136000000002E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -1286,8 +1390,11 @@
       <c r="H37">
         <v>7.8076669840000001E-2</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K37">
+        <v>4.0734589999999998E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -1306,8 +1413,11 @@
       <c r="H38">
         <v>7.806480214E-2</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K38">
+        <v>4.1047083999999996E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -1326,8 +1436,11 @@
       <c r="H39">
         <v>8.1796734119999895E-2</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K39">
+        <v>4.0811668000000009E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -1346,8 +1459,11 @@
       <c r="H40" s="2">
         <v>2.8549580000000001E-5</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K40">
+        <v>5.4144294000000003E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -1366,8 +1482,11 @@
       <c r="H41" s="2">
         <v>2.7684240000000001E-5</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K41">
+        <v>5.2100810000000001E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>41</v>
       </c>
@@ -1386,8 +1505,11 @@
       <c r="H42" s="2">
         <v>2.0396439999999901E-5</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K42">
+        <v>5.1429767999999999E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>42</v>
       </c>
@@ -1406,8 +1528,11 @@
       <c r="H43">
         <v>4.8438676959999899E-2</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K43">
+        <v>5.4535816000000001E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>43</v>
       </c>
@@ -1426,8 +1551,11 @@
       <c r="H44">
         <v>3.8956613700000003E-2</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K44">
+        <v>5.5146069999999995E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>44</v>
       </c>
@@ -1446,8 +1574,11 @@
       <c r="H45">
         <v>4.1313744479999998E-2</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K45">
+        <v>5.4049389999999992E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>45</v>
       </c>
@@ -1466,8 +1597,11 @@
       <c r="H46">
         <v>1.3609141785799901</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K46">
+        <v>5.5638765999999999E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>46</v>
       </c>
@@ -1486,8 +1620,11 @@
       <c r="H47">
         <v>1.23728365578</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K47">
+        <v>5.3607398000000001E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>47</v>
       </c>
@@ -1506,8 +1643,11 @@
       <c r="H48">
         <v>1.21835427683999</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K48">
+        <v>5.2173544000000006E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>48</v>
       </c>
@@ -1526,8 +1666,11 @@
       <c r="H49" s="2">
         <v>3.8763999999999997E-5</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K49">
+        <v>3.8839354E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>49</v>
       </c>
@@ -1546,8 +1689,11 @@
       <c r="H50" s="2">
         <v>4.8773879999999901E-5</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K50">
+        <v>4.0439513999999998E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>50</v>
       </c>
@@ -1566,8 +1712,11 @@
       <c r="H51" s="2">
         <v>5.0324279999999899E-5</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K51">
+        <v>3.8420462000000001E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>51</v>
       </c>
@@ -1586,8 +1735,11 @@
       <c r="H52">
         <v>6.9941663900000006E-2</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K52">
+        <v>4.2701772000000009E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>52</v>
       </c>
@@ -1606,8 +1758,11 @@
       <c r="H53">
         <v>6.6037970539999893E-2</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K53">
+        <v>4.5588212000000003E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>53</v>
       </c>
@@ -1617,8 +1772,11 @@
       <c r="D54">
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K54">
+        <v>4.3485873999999994E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>54</v>
       </c>
@@ -1628,8 +1786,11 @@
       <c r="D55">
         <v>16</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K55">
+        <v>4.4230588E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>55</v>
       </c>
@@ -1639,8 +1800,11 @@
       <c r="D56">
         <v>16</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K56">
+        <v>4.3643681999999996E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>56</v>
       </c>
@@ -1649,6 +1813,9 @@
       </c>
       <c r="D57">
         <v>16</v>
+      </c>
+      <c r="K57">
+        <v>4.4585201999999997E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1661,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE147AB4-93A1-4224-A52F-043C7AD8859B}">
   <dimension ref="B1:L57"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1671,15 +1838,17 @@
     <col min="3" max="3" width="13.88671875" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -1704,10 +1873,10 @@
         <v>60</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
@@ -1728,6 +1897,9 @@
       </c>
       <c r="H3" s="2">
         <v>5.0696548000000001E-3</v>
+      </c>
+      <c r="K3">
+        <v>0.58662594620000008</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
@@ -1749,6 +1921,9 @@
       <c r="H4" s="2">
         <v>5.32227457999999E-3</v>
       </c>
+      <c r="K4">
+        <v>0.59564800360000003</v>
+      </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -1769,6 +1944,9 @@
       <c r="H5" s="2">
         <v>6.2013390599999999E-3</v>
       </c>
+      <c r="K5">
+        <v>0.58060226079999999</v>
+      </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -1789,6 +1967,9 @@
       <c r="H6">
         <v>4.0904141739999997E-2</v>
       </c>
+      <c r="K6">
+        <v>0.57893442499999992</v>
+      </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -1809,6 +1990,9 @@
       <c r="H7">
         <v>9.61732805E-2</v>
       </c>
+      <c r="K7">
+        <v>0.57935043919999996</v>
+      </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
@@ -1829,6 +2013,9 @@
       <c r="H8">
         <v>6.6781945299999895E-2</v>
       </c>
+      <c r="K8">
+        <v>0.59767893179999998</v>
+      </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
@@ -1848,6 +2035,9 @@
       </c>
       <c r="H9">
         <v>0.49750794745999999</v>
+      </c>
+      <c r="K9">
+        <v>0.57504232760000007</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -1869,6 +2059,9 @@
       <c r="H10">
         <v>0.26222596496</v>
       </c>
+      <c r="K10">
+        <v>0.58018073440000006</v>
+      </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
@@ -1889,6 +2082,9 @@
       <c r="H11">
         <v>0.46647592725999998</v>
       </c>
+      <c r="K11">
+        <v>0.58513556839999992</v>
+      </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -1909,6 +2105,9 @@
       <c r="H12">
         <v>7.3398038919999894E-2</v>
       </c>
+      <c r="K12">
+        <v>0.6151272296000001</v>
+      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
@@ -1929,6 +2128,9 @@
       <c r="H13">
         <v>0.117171630979999</v>
       </c>
+      <c r="K13">
+        <v>0.60849440259999998</v>
+      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -1949,6 +2151,9 @@
       <c r="H14">
         <v>4.5263969739999903E-2</v>
       </c>
+      <c r="K14">
+        <v>0.61084418560000009</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
@@ -1969,6 +2174,9 @@
       <c r="H15">
         <v>7.7530737077999996</v>
       </c>
+      <c r="K15">
+        <v>0.60972718720000008</v>
+      </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -1989,8 +2197,11 @@
       <c r="H16">
         <v>5.8970220660199901</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>0.62532689959999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -2009,8 +2220,11 @@
       <c r="H17">
         <v>6.4239563367199999</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <v>0.60839207200000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -2029,8 +2243,11 @@
       <c r="H18">
         <v>30.370443534379898</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>0.60294468899999998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -2049,8 +2266,11 @@
       <c r="H19">
         <v>62.062277821779901</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>0.62043525360000007</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -2069,8 +2289,11 @@
       <c r="H20">
         <v>31.666343097759999</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>0.62141416300000007</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>20</v>
       </c>
@@ -2089,8 +2312,11 @@
       <c r="H21">
         <v>0.18082493127999999</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>0.91561420859999987</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -2109,8 +2335,11 @@
       <c r="H22">
         <v>0.75351090395999898</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K22">
+        <v>0.92705632559999995</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -2129,8 +2358,11 @@
       <c r="H23">
         <v>0.24073645590000001</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K23">
+        <v>0.93054749339999998</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -2149,8 +2381,11 @@
       <c r="H24">
         <v>6.6725374729600002</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K24">
+        <v>0.92683057499999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -2169,8 +2404,11 @@
       <c r="H25">
         <v>23.604746588859999</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K25">
+        <v>0.92396037780000007</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>25</v>
       </c>
@@ -2180,8 +2418,11 @@
       <c r="D26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>0.91680164919999996</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -2191,8 +2432,11 @@
       <c r="D27">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>0.91455887980000006</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -2202,8 +2446,11 @@
       <c r="D28">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K28">
+        <v>0.92582346739999988</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -2213,8 +2460,11 @@
       <c r="D29">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K29">
+        <v>0.90954062120000001</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -2233,8 +2483,11 @@
       <c r="H31" s="2">
         <v>5.5116003999999895E-4</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K31">
+        <v>0.58994035239999998</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -2253,8 +2506,11 @@
       <c r="H32" s="2">
         <v>7.0128569999999997E-4</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K32">
+        <v>0.58220385139999997</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -2273,8 +2529,11 @@
       <c r="H33" s="2">
         <v>7.3267213999999995E-4</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K33">
+        <v>0.60370893660000002</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -2293,8 +2552,11 @@
       <c r="H34">
         <v>1.42274894599999E-2</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K34">
+        <v>0.58489644379999994</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -2313,8 +2575,11 @@
       <c r="H35">
         <v>2.0724687459999998E-2</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K35">
+        <v>0.58463533519999999</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -2333,8 +2598,11 @@
       <c r="H36">
         <v>1.6236867320000001E-2</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K36">
+        <v>0.60728247639999999</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -2353,8 +2621,11 @@
       <c r="H37">
         <v>0.116301179239999</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K37">
+        <v>0.58253205220000004</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -2373,8 +2644,11 @@
       <c r="H38">
         <v>0.12504765564</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K38">
+        <v>0.58252015300000004</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -2393,8 +2667,11 @@
       <c r="H39">
         <v>0.122053745079999</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K39">
+        <v>0.58043706859999999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -2413,8 +2690,11 @@
       <c r="H40" s="2">
         <v>2.7587401399999899E-3</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K40">
+        <v>0.61043776400000005</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -2433,8 +2713,11 @@
       <c r="H41" s="2">
         <v>4.4973114200000004E-3</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K41">
+        <v>0.60774840999999991</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>41</v>
       </c>
@@ -2453,8 +2736,11 @@
       <c r="H42" s="2">
         <v>4.6491934200000003E-3</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K42">
+        <v>0.61040038519999995</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>42</v>
       </c>
@@ -2473,8 +2759,11 @@
       <c r="H43">
         <v>0.14510178539999999</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K43">
+        <v>0.61419026980000002</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>43</v>
       </c>
@@ -2493,8 +2782,11 @@
       <c r="H44">
         <v>0.14302093901999999</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K44">
+        <v>0.62029711619999994</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>44</v>
       </c>
@@ -2513,8 +2805,11 @@
       <c r="H45">
         <v>0.172773514179999</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K45">
+        <v>0.6098337304</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>45</v>
       </c>
@@ -2533,8 +2828,11 @@
       <c r="H46">
         <v>2.0340562132599902</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K46">
+        <v>0.61400893979999993</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>46</v>
       </c>
@@ -2553,8 +2851,11 @@
       <c r="H47">
         <v>2.1219118204399998</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K47">
+        <v>0.60232572159999997</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>47</v>
       </c>
@@ -2573,8 +2874,11 @@
       <c r="H48">
         <v>2.11668509493999</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K48">
+        <v>0.60812195759999998</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>48</v>
       </c>
@@ -2593,8 +2897,11 @@
       <c r="H49">
         <v>5.6333308999999996E-3</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K49">
+        <v>0.93289946040000005</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>49</v>
       </c>
@@ -2613,8 +2920,11 @@
       <c r="H50">
         <v>5.9055875000000001E-3</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K50">
+        <v>0.92527228519999993</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>50</v>
       </c>
@@ -2633,8 +2943,11 @@
       <c r="H51">
         <v>5.2234269599999899E-3</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K51">
+        <v>0.92407379079999996</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>51</v>
       </c>
@@ -2653,8 +2966,11 @@
       <c r="H52">
         <v>0.23102593653999901</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K52">
+        <v>0.9413188802000001</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>52</v>
       </c>
@@ -2673,8 +2989,11 @@
       <c r="H53">
         <v>0.26960134466000002</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K53">
+        <v>0.90655656619999991</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>53</v>
       </c>
@@ -2684,8 +3003,11 @@
       <c r="D54">
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K54">
+        <v>0.9267903796000001</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>54</v>
       </c>
@@ -2695,8 +3017,11 @@
       <c r="D55">
         <v>16</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K55">
+        <v>0.91296492279999997</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>55</v>
       </c>
@@ -2706,8 +3031,11 @@
       <c r="D56">
         <v>16</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K56">
+        <v>0.92770335300000006</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>56</v>
       </c>
@@ -2716,6 +3044,9 @@
       </c>
       <c r="D57">
         <v>16</v>
+      </c>
+      <c r="K57">
+        <v>0.90154461699999988</v>
       </c>
     </row>
   </sheetData>
@@ -2728,8 +3059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D026784-D940-4903-8CB7-2720278E37DA}">
   <dimension ref="B1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2738,15 +3069,17 @@
     <col min="3" max="3" width="13.88671875" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -2771,10 +3104,10 @@
         <v>60</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
@@ -2795,6 +3128,9 @@
       </c>
       <c r="H3" s="2">
         <v>4.1356929600000003E-3</v>
+      </c>
+      <c r="K3">
+        <v>1.1401731199999999E-2</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
@@ -2816,6 +3152,9 @@
       <c r="H4" s="2">
         <v>3.2725067600000001E-3</v>
       </c>
+      <c r="K4">
+        <v>1.15930258E-2</v>
+      </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -2836,6 +3175,9 @@
       <c r="H5" s="2">
         <v>7.4947991400000002E-3</v>
       </c>
+      <c r="K5">
+        <v>1.14035232E-2</v>
+      </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -2856,6 +3198,9 @@
       <c r="H6">
         <v>0.35905098586</v>
       </c>
+      <c r="K6">
+        <v>2.9874872399999995E-2</v>
+      </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -2876,6 +3221,9 @@
       <c r="H7">
         <v>0.22416156273999999</v>
       </c>
+      <c r="K7">
+        <v>2.9895556600000001E-2</v>
+      </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
@@ -2896,6 +3244,9 @@
       <c r="H8">
         <v>0.348906167759999</v>
       </c>
+      <c r="K8">
+        <v>2.9972331200000001E-2</v>
+      </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
@@ -2915,6 +3266,9 @@
       </c>
       <c r="H9">
         <v>4.5455594814999998</v>
+      </c>
+      <c r="K9">
+        <v>5.3499613799999998E-2</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -2936,6 +3290,9 @@
       <c r="H10">
         <v>3.1230741166399998</v>
       </c>
+      <c r="K10">
+        <v>5.3582124599999989E-2</v>
+      </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
@@ -2956,6 +3313,9 @@
       <c r="H11">
         <v>3.1659101450599998</v>
       </c>
+      <c r="K11">
+        <v>5.3457578800000002E-2</v>
+      </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -2976,6 +3336,9 @@
       <c r="H12">
         <v>0.19788447099999901</v>
       </c>
+      <c r="K12">
+        <v>5.3403133800000002E-2</v>
+      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
@@ -2996,6 +3359,9 @@
       <c r="H13">
         <v>0.15005009752000001</v>
       </c>
+      <c r="K13">
+        <v>5.3859272399999991E-2</v>
+      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -3016,6 +3382,9 @@
       <c r="H14">
         <v>0.14273448331999899</v>
       </c>
+      <c r="K14">
+        <v>5.3676924599999995E-2</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
@@ -3036,6 +3405,9 @@
       <c r="H15">
         <v>21.77143943486</v>
       </c>
+      <c r="K15">
+        <v>0.2262258298</v>
+      </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -3056,8 +3428,11 @@
       <c r="H16">
         <v>17.604372304519998</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>0.23694273020000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -3076,8 +3451,11 @@
       <c r="H17">
         <v>12.861388567659899</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <v>0.22788959760000002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -3096,8 +3474,11 @@
       <c r="H18">
         <v>191.482833445599</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>1.5174602668000001</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -3116,8 +3497,11 @@
       <c r="H19">
         <v>170.114718766539</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>1.5304654605999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -3136,8 +3520,11 @@
       <c r="H20">
         <v>147.98593053757901</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>1.5019303646</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>20</v>
       </c>
@@ -3156,8 +3543,11 @@
       <c r="H21">
         <v>0.38844534936000003</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>0.16882178959999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -3176,8 +3566,11 @@
       <c r="H22">
         <v>0.2332781498</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K22">
+        <v>0.17171642619999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -3196,8 +3589,11 @@
       <c r="H23">
         <v>0.30746786787999902</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K23">
+        <v>0.17301536080000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -3216,8 +3612,11 @@
       <c r="H24">
         <v>40.923313784379999</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K24">
+        <v>0.95210933580000001</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -3236,8 +3635,11 @@
       <c r="H25">
         <v>58.728886067859897</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K25">
+        <v>0.93855278319999991</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>25</v>
       </c>
@@ -3247,8 +3649,11 @@
       <c r="D26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>1.0737185376</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -3258,8 +3663,11 @@
       <c r="D27">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>1.2130380584</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -3269,8 +3677,11 @@
       <c r="D28">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K28">
+        <v>1.228560168</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -3280,8 +3691,11 @@
       <c r="D29">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K29">
+        <v>1.2376574236</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -3300,8 +3714,11 @@
       <c r="H31" s="2">
         <v>1.3453178400000001E-3</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K31">
+        <v>1.1448608999999998E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -3320,8 +3737,11 @@
       <c r="H32" s="2">
         <v>1.04205698E-3</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K32">
+        <v>1.1389925799999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -3340,8 +3760,11 @@
       <c r="H33" s="2">
         <v>1.3702455199999901E-3</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K33">
+        <v>1.15276094E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -3360,8 +3783,11 @@
       <c r="H34">
         <v>5.8049505539999997E-2</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K34">
+        <v>2.9916441000000005E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -3380,8 +3806,11 @@
       <c r="H35">
         <v>7.568579298E-2</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K35">
+        <v>2.9986563000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -3400,8 +3829,11 @@
       <c r="H36">
         <v>7.9085868500000003E-2</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K36">
+        <v>3.0065096400000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -3420,8 +3852,11 @@
       <c r="H37">
         <v>1.1132623243599999</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K37">
+        <v>5.3867455200000004E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -3440,8 +3875,11 @@
       <c r="H38">
         <v>1.09470546585999</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K38">
+        <v>5.3786152199999993E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -3460,8 +3898,11 @@
       <c r="H39">
         <v>1.10148578874</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K39">
+        <v>5.3920919199999993E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -3480,8 +3921,11 @@
       <c r="H40" s="2">
         <v>7.4134531999999996E-3</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K40">
+        <v>5.3311936400000003E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -3500,8 +3944,11 @@
       <c r="H41" s="2">
         <v>8.2336566799999997E-3</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K41">
+        <v>5.42479056E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>41</v>
       </c>
@@ -3520,8 +3967,11 @@
       <c r="H42" s="2">
         <v>7.1501492199999902E-3</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K42">
+        <v>5.3669263599999996E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>42</v>
       </c>
@@ -3540,8 +3990,11 @@
       <c r="H43">
         <v>0.75729544676000005</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K43">
+        <v>0.229725437</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>43</v>
       </c>
@@ -3560,8 +4013,11 @@
       <c r="H44">
         <v>0.66982079175999998</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K44">
+        <v>0.23091449260000002</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>44</v>
       </c>
@@ -3580,8 +4036,11 @@
       <c r="H45">
         <v>0.689804475279999</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K45">
+        <v>0.22994558999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>45</v>
       </c>
@@ -3600,8 +4059,11 @@
       <c r="H46">
         <v>11.41930225728</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K46">
+        <v>1.5702458334</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>46</v>
       </c>
@@ -3620,8 +4082,11 @@
       <c r="H47">
         <v>10.8113482497599</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K47">
+        <v>1.4952725331999999</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>47</v>
       </c>
@@ -3640,8 +4105,11 @@
       <c r="H48">
         <v>11.70780505428</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K48">
+        <v>1.5027987166000001</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>48</v>
       </c>
@@ -3660,8 +4128,11 @@
       <c r="H49">
         <v>1.3292112599999999E-2</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K49">
+        <v>0.1795483044</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>49</v>
       </c>
@@ -3680,8 +4151,11 @@
       <c r="H50">
         <v>1.21706141399999E-2</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K50">
+        <v>0.1698281864</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>50</v>
       </c>
@@ -3700,8 +4174,11 @@
       <c r="H51">
         <v>1.149454862E-2</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K51">
+        <v>0.16888884240000002</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>51</v>
       </c>
@@ -3720,8 +4197,11 @@
       <c r="H52">
         <v>1.5219997734199999</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K52">
+        <v>0.92710600919999986</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>52</v>
       </c>
@@ -3740,8 +4220,11 @@
       <c r="H53">
         <v>1.3638920507800001</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K53">
+        <v>1.1124177218</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>53</v>
       </c>
@@ -3751,8 +4234,11 @@
       <c r="D54">
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K54">
+        <v>1.0662151376</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>54</v>
       </c>
@@ -3762,8 +4248,11 @@
       <c r="D55">
         <v>16</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K55">
+        <v>1.7103487042000001</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>55</v>
       </c>
@@ -3773,8 +4262,11 @@
       <c r="D56">
         <v>16</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K56">
+        <v>1.4423819873999999</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>56</v>
       </c>
@@ -3783,6 +4275,9 @@
       </c>
       <c r="D57">
         <v>16</v>
+      </c>
+      <c r="K57">
+        <v>1.8803625462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Edge Addition to results table
</commit_message>
<xml_diff>
--- a/Data/Scenarios/Graph List and Stats.xlsx
+++ b/Data/Scenarios/Graph List and Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marto\git\Algos_Assignment1\Data\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD4E513-561C-427E-B5FF-4339AACBBF7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC38DF5-1489-4BEF-A8E0-78221D19D8C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22752" yWindow="192" windowWidth="21252" windowHeight="13608" activeTab="2" xr2:uid="{61CBB812-40D1-44A3-AFF3-2B0F76CA3C04}"/>
+    <workbookView xWindow="24576" yWindow="156" windowWidth="21252" windowHeight="13608" xr2:uid="{61CBB812-40D1-44A3-AFF3-2B0F76CA3C04}"/>
   </bookViews>
   <sheets>
     <sheet name="AdjList" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="74">
   <si>
     <t>Filename</t>
   </si>
@@ -237,6 +237,27 @@
   </si>
   <si>
     <t>deleting 100 vertices (avg. time of total 5 iterations)</t>
+  </si>
+  <si>
+    <t>adding 10,000 edges (avg. of total 5 iterations)</t>
+  </si>
+  <si>
+    <t>Edge Additions</t>
+  </si>
+  <si>
+    <t>Scale-Free</t>
+  </si>
+  <si>
+    <t>Erdos</t>
+  </si>
+  <si>
+    <t>Graph Type</t>
+  </si>
+  <si>
+    <t>deleting 100 edges (avg. of total 5 iterations)</t>
+  </si>
+  <si>
+    <t>Edge Deletions</t>
   </si>
 </sst>
 </file>
@@ -280,10 +301,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,34 +622,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D71CDE3-7DBD-462C-93FC-85AE65D9340E}">
-  <dimension ref="B1:L57"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.21875" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="11" max="11" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.44140625" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
     <col min="12" max="12" width="21.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,8 +691,17 @@
       <c r="L2" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -679,8 +726,14 @@
       <c r="L3">
         <v>0.13432737339999998</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>8.3807535999999988E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -705,8 +758,14 @@
       <c r="L4">
         <v>0.11682669319999998</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>8.2867992000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -731,8 +790,14 @@
       <c r="L5">
         <v>0.15311848759999996</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>8.7069480000000008E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -757,8 +822,14 @@
       <c r="L6">
         <v>0.13317663839999999</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>1.0384794399999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -783,8 +854,14 @@
       <c r="L7">
         <v>0.11746011720000001</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>1.0128469399999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -809,8 +886,14 @@
       <c r="L8">
         <v>0.13912788540000001</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M8">
+        <v>1.02744464E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -835,8 +918,14 @@
       <c r="L9">
         <v>0.13818872540000002</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M9">
+        <v>1.2140006599999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -861,8 +950,14 @@
       <c r="L10">
         <v>0.1435946538</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M10">
+        <v>1.2265112200000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -887,8 +982,14 @@
       <c r="L11">
         <v>0.14413307140000001</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M11">
+        <v>1.2146577E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -913,8 +1014,14 @@
       <c r="L12">
         <v>0.35413641479999997</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M12">
+        <v>4.4773660000000009E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -939,8 +1046,14 @@
       <c r="L13">
         <v>0.32794630899999999</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <v>4.3611811999999996E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -965,8 +1078,14 @@
       <c r="L14">
         <v>0.32883370219999997</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M14">
+        <v>4.5003481999999996E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -991,8 +1110,14 @@
       <c r="L15">
         <v>0.33321776679999998</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M15">
+        <v>7.3912489999999999E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -1017,8 +1142,14 @@
       <c r="L16">
         <v>0.39692611379999998</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M16">
+        <v>7.6986950000000002E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -1043,8 +1174,14 @@
       <c r="L17">
         <v>0.40045458319999999</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M17">
+        <v>7.528757799999999E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -1069,8 +1206,14 @@
       <c r="L18">
         <v>0.40600428540000005</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M18">
+        <v>1.22091396E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -1095,8 +1238,14 @@
       <c r="L19">
         <v>0.38220546500000002</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <v>1.0606054600000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -1121,8 +1270,14 @@
       <c r="L20">
         <v>0.44760460079999997</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M20">
+        <v>1.0563634799999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
@@ -1147,8 +1302,14 @@
       <c r="L21">
         <v>0.3771424458</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M21">
+        <v>6.8569162000000003E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -1173,8 +1334,14 @@
       <c r="L22">
         <v>0.2332328592</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M22">
+        <v>5.6390249999999998E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -1199,8 +1366,14 @@
       <c r="L23">
         <v>0.33083184499999996</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M23">
+        <v>6.4650281999999986E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -1225,8 +1398,14 @@
       <c r="L24">
         <v>0.42947305779999995</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M24">
+        <v>9.123151799999998E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -1251,8 +1430,14 @@
       <c r="L25">
         <v>0.4661468082000001</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M25">
+        <v>8.9317818E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
@@ -1268,8 +1453,14 @@
       <c r="L26">
         <v>0.40356881979999998</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M26">
+        <v>1.0180942200000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -1285,8 +1476,14 @@
       <c r="L27">
         <v>1.1231289108</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M27">
+        <v>1.83579548E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -1302,8 +1499,14 @@
       <c r="L28">
         <v>1.150247606</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M28">
+        <v>2.2744319800000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -1319,8 +1522,14 @@
       <c r="L29">
         <v>1.2165469834</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M29">
+        <v>1.8444252799999998E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -1345,8 +1554,14 @@
       <c r="L31">
         <v>0.1100308414</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M31">
+        <v>8.3659453999999998E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -1371,8 +1586,14 @@
       <c r="L32">
         <v>0.11036385980000001</v>
       </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M32">
+        <v>8.8110241999999998E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -1397,8 +1618,14 @@
       <c r="L33">
         <v>0.13813482100000002</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M33">
+        <v>8.4167651999999989E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -1423,8 +1650,14 @@
       <c r="L34">
         <v>0.18146999619999998</v>
       </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M34">
+        <v>1.0793509199999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -1449,8 +1682,14 @@
       <c r="L35">
         <v>0.11351082059999999</v>
       </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M35">
+        <v>1.0817901E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -1475,8 +1714,14 @@
       <c r="L36">
         <v>0.1605168092</v>
       </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M36">
+        <v>1.03197588E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -1501,8 +1746,14 @@
       <c r="L37">
         <v>0.18628030579999999</v>
       </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M37">
+        <v>1.2785229400000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -1527,8 +1778,14 @@
       <c r="L38">
         <v>0.13070518980000001</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M38">
+        <v>1.28941426E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -1553,8 +1810,14 @@
       <c r="L39">
         <v>0.12592313800000002</v>
       </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M39">
+        <v>1.2794812999999999E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -1579,8 +1842,14 @@
       <c r="L40">
         <v>0.2864000988</v>
       </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M40">
+        <v>5.0359865999999994E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -1605,8 +1874,14 @@
       <c r="L41">
         <v>0.29310883000000004</v>
       </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M41">
+        <v>4.7782700000000003E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
@@ -1631,8 +1906,14 @@
       <c r="L42">
         <v>0.30067468380000001</v>
       </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M42">
+        <v>5.0427189999999993E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
@@ -1657,8 +1938,14 @@
       <c r="L43">
         <v>0.31160468979999995</v>
       </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M43">
+        <v>7.3908035999999998E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
@@ -1683,8 +1970,14 @@
       <c r="L44">
         <v>0.31272636640000001</v>
       </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M44">
+        <v>7.3493641999999998E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
       <c r="B45" t="s">
         <v>44</v>
       </c>
@@ -1709,8 +2002,14 @@
       <c r="L45">
         <v>0.29171352700000003</v>
       </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M45">
+        <v>7.3294559999999998E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
@@ -1735,8 +2034,14 @@
       <c r="L46">
         <v>0.28971804680000002</v>
       </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M46">
+        <v>1.0357852800000001E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
@@ -1761,8 +2066,14 @@
       <c r="L47">
         <v>0.29276012480000002</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M47">
+        <v>1.1232658400000001E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
@@ -1787,8 +2098,14 @@
       <c r="L48">
         <v>0.29452768339999996</v>
       </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M48">
+        <v>1.1294334999999999E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
@@ -1813,8 +2130,14 @@
       <c r="L49">
         <v>0.31950814280000001</v>
       </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M49">
+        <v>6.0550691999999998E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
@@ -1839,8 +2162,14 @@
       <c r="L50">
         <v>0.29901791119999999</v>
       </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M50">
+        <v>6.4120845999999995E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
@@ -1865,8 +2194,14 @@
       <c r="L51">
         <v>0.35236761420000001</v>
       </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M51">
+        <v>5.7054139999999989E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
@@ -1891,8 +2226,14 @@
       <c r="L52">
         <v>0.41743242899999994</v>
       </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M52">
+        <v>9.5543725999999995E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
@@ -1917,8 +2258,14 @@
       <c r="L53">
         <v>0.36986134739999998</v>
       </c>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M53">
+        <v>9.6892556000000001E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
       <c r="B54" t="s">
         <v>53</v>
       </c>
@@ -1934,8 +2281,14 @@
       <c r="L54">
         <v>0.37822567320000006</v>
       </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M54">
+        <v>8.6676488000000003E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
       <c r="B55" t="s">
         <v>54</v>
       </c>
@@ -1951,8 +2304,14 @@
       <c r="L55">
         <v>1.0909963616</v>
       </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M55">
+        <v>2.0723615799999998E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
       <c r="B56" t="s">
         <v>55</v>
       </c>
@@ -1968,8 +2327,14 @@
       <c r="L56">
         <v>1.1980403369999999</v>
       </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M56">
+        <v>1.8357725199999998E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>70</v>
+      </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
@@ -1984,6 +2349,9 @@
       </c>
       <c r="L57">
         <v>1.2431462602000001</v>
+      </c>
+      <c r="M57">
+        <v>2.0861954600000003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1994,34 +2362,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE147AB4-93A1-4224-A52F-043C7AD8859B}">
-  <dimension ref="B1:L57"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31:L57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.44140625" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="11" max="11" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.77734375" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
     <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="14" max="14" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2049,8 +2431,17 @@
       <c r="L2" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -2075,8 +2466,14 @@
       <c r="L3">
         <v>8.4116568000000003E-3</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>2.8862903999999998E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2101,8 +2498,14 @@
       <c r="L4">
         <v>8.3474979999999983E-3</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>3.1253242000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2127,8 +2530,14 @@
       <c r="L5">
         <v>8.4190347999999991E-3</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>2.8668409999999997E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2153,8 +2562,14 @@
       <c r="L6">
         <v>8.7117679999999999E-3</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>2.7152946000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -2179,8 +2594,14 @@
       <c r="L7">
         <v>8.6729943999999982E-3</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>2.8800506000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -2205,8 +2626,14 @@
       <c r="L8">
         <v>8.8367237999999997E-3</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M8">
+        <v>2.8963023999999996E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -2231,8 +2658,14 @@
       <c r="L9">
         <v>8.9190956000000012E-3</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M9">
+        <v>2.9429674E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -2257,8 +2690,14 @@
       <c r="L10">
         <v>8.753884600000001E-3</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M10">
+        <v>2.9098943999999998E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -2283,8 +2722,14 @@
       <c r="L11">
         <v>8.6177023999999998E-3</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M11">
+        <v>2.6162008000000002E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -2309,8 +2754,14 @@
       <c r="L12">
         <v>2.9481749000000002E-2</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M12">
+        <v>3.5555404E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -2335,8 +2786,14 @@
       <c r="L13">
         <v>3.0139562200000004E-2</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <v>3.5390292000000005E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -2361,8 +2818,14 @@
       <c r="L14">
         <v>2.8999482E-2</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M14">
+        <v>3.5637552000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -2387,8 +2850,14 @@
       <c r="L15">
         <v>2.8881893000000002E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M15">
+        <v>4.2361585999999996E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -2413,8 +2882,14 @@
       <c r="L16">
         <v>2.9362489600000003E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M16">
+        <v>4.3571832000000007E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -2439,8 +2914,14 @@
       <c r="L17">
         <v>2.9575663800000002E-2</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M17">
+        <v>4.5842410000000002E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -2465,8 +2946,14 @@
       <c r="L18">
         <v>3.0236952399999999E-2</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M18">
+        <v>4.4476558000000003E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -2491,8 +2978,14 @@
       <c r="L19">
         <v>2.9551223599999999E-2</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <v>4.4124348000000009E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -2517,8 +3010,14 @@
       <c r="L20">
         <v>2.9946947599999996E-2</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M20">
+        <v>4.4733486000000005E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
@@ -2543,8 +3042,14 @@
       <c r="L21">
         <v>4.6036894799999999E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M21">
+        <v>5.1049787999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -2569,8 +3074,14 @@
       <c r="L22">
         <v>4.445447680000001E-2</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M22">
+        <v>5.0402588E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -2595,8 +3106,14 @@
       <c r="L23">
         <v>4.7763275000000001E-2</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M23">
+        <v>5.0366209999999998E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -2621,8 +3138,14 @@
       <c r="L24">
         <v>4.8630516200000001E-2</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M24">
+        <v>5.4801090000000004E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -2647,8 +3170,14 @@
       <c r="L25">
         <v>4.3949066199999998E-2</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M25">
+        <v>5.7253286000000002E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
@@ -2664,8 +3193,14 @@
       <c r="L26">
         <v>4.9612748800000002E-2</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M26">
+        <v>4.9378644000000003E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -2681,8 +3216,14 @@
       <c r="L27">
         <v>4.9514213599999995E-2</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M27">
+        <v>5.5507638000000005E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -2698,8 +3239,14 @@
       <c r="L28">
         <v>4.7100343599999997E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M28">
+        <v>6.2502383999999992E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -2715,8 +3262,14 @@
       <c r="L29">
         <v>4.3880430600000006E-2</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M29">
+        <v>5.9546513999999993E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -2741,8 +3294,14 @@
       <c r="L31">
         <v>8.4604868000000017E-3</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M31">
+        <v>2.8994292000000003E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -2767,8 +3326,14 @@
       <c r="L32">
         <v>8.4638561999999997E-3</v>
       </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M32">
+        <v>2.8637768E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -2793,8 +3358,14 @@
       <c r="L33">
         <v>8.3724869999999996E-3</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M33">
+        <v>2.9406817999999999E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -2819,8 +3390,14 @@
       <c r="L34">
         <v>8.6066038000000011E-3</v>
       </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M34">
+        <v>2.9363385999999999E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -2845,8 +3422,14 @@
       <c r="L35">
         <v>8.7086694000000006E-3</v>
       </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M35">
+        <v>2.8112326000000001E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -2871,8 +3454,14 @@
       <c r="L36">
         <v>8.6387327999999999E-3</v>
       </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M36">
+        <v>2.8126665999999999E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -2897,8 +3486,14 @@
       <c r="L37">
         <v>8.8660400000000004E-3</v>
       </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M37">
+        <v>2.8208598000000001E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -2923,8 +3518,14 @@
       <c r="L38">
         <v>8.7987114000000009E-3</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M38">
+        <v>3.1190205999999999E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -2949,8 +3550,14 @@
       <c r="L39">
         <v>8.9113123999999995E-3</v>
       </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M39">
+        <v>2.6502381999999997E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -2975,8 +3582,14 @@
       <c r="L40">
         <v>2.8623563400000003E-2</v>
       </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M40">
+        <v>3.5016261999999999E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -3001,8 +3614,14 @@
       <c r="L41">
         <v>2.8761465399999998E-2</v>
       </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M41">
+        <v>3.5930391999999998E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
@@ -3027,8 +3646,14 @@
       <c r="L42">
         <v>2.8447589000000002E-2</v>
       </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M42">
+        <v>3.5827513999999996E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
@@ -3053,8 +3678,14 @@
       <c r="L43">
         <v>2.87392572E-2</v>
       </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M43">
+        <v>4.3924413999999997E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
@@ -3079,8 +3710,14 @@
       <c r="L44">
         <v>2.9272065000000003E-2</v>
       </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M44">
+        <v>4.5679278000000005E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
       <c r="B45" t="s">
         <v>44</v>
       </c>
@@ -3105,8 +3742,14 @@
       <c r="L45">
         <v>2.9076954799999999E-2</v>
       </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M45">
+        <v>4.6449940000000004E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
@@ -3131,8 +3774,14 @@
       <c r="L46">
         <v>2.9397026799999997E-2</v>
       </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M46">
+        <v>4.6782552000000002E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
@@ -3157,8 +3806,14 @@
       <c r="L47">
         <v>2.9821098000000001E-2</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M47">
+        <v>4.5673904000000003E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
@@ -3183,8 +3838,14 @@
       <c r="L48">
         <v>3.0199749200000004E-2</v>
       </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M48">
+        <v>4.7409218000000006E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
@@ -3209,8 +3870,14 @@
       <c r="L49">
         <v>4.6451986200000003E-2</v>
       </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M49">
+        <v>4.9135204000000004E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
@@ -3235,8 +3902,14 @@
       <c r="L50">
         <v>4.1719389600000004E-2</v>
       </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M50">
+        <v>4.9549842E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
@@ -3261,8 +3934,14 @@
       <c r="L51">
         <v>4.7375330400000006E-2</v>
       </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M51">
+        <v>5.3172430000000001E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
@@ -3287,8 +3966,14 @@
       <c r="L52">
         <v>4.6011317400000008E-2</v>
       </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M52">
+        <v>5.1234062000000014E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
@@ -3313,8 +3998,14 @@
       <c r="L53">
         <v>4.5068810600000002E-2</v>
       </c>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M53">
+        <v>5.5103132000000003E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
       <c r="B54" t="s">
         <v>53</v>
       </c>
@@ -3330,8 +4021,14 @@
       <c r="L54">
         <v>4.9042818000000002E-2</v>
       </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M54">
+        <v>5.6261578E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
       <c r="B55" t="s">
         <v>54</v>
       </c>
@@ -3347,8 +4044,14 @@
       <c r="L55">
         <v>4.7415108400000003E-2</v>
       </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M55">
+        <v>5.5034229999999995E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
       <c r="B56" t="s">
         <v>55</v>
       </c>
@@ -3364,8 +4067,14 @@
       <c r="L56">
         <v>4.5402461200000008E-2</v>
       </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M56">
+        <v>6.1231876000000006E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>70</v>
+      </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
@@ -3380,6 +4089,9 @@
       </c>
       <c r="L57">
         <v>4.4885005800000002E-2</v>
+      </c>
+      <c r="M57">
+        <v>6.1870375999999996E-3</v>
       </c>
     </row>
   </sheetData>
@@ -3390,34 +4102,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D026784-D940-4903-8CB7-2720278E37DA}">
-  <dimension ref="B1:L57"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31:L57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.109375" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="11" max="11" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" customWidth="1"/>
     <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.88671875" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3445,8 +4171,17 @@
       <c r="L2" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -3471,8 +4206,14 @@
       <c r="L3">
         <v>4.7499912199999994E-2</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>0.10495889680000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -3497,8 +4238,14 @@
       <c r="L4">
         <v>4.7319866200000005E-2</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>0.10670013760000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -3523,8 +4270,14 @@
       <c r="L5">
         <v>4.6682723999999995E-2</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>0.10427209340000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -3549,8 +4302,14 @@
       <c r="L6">
         <v>0.1049426456</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>0.1029034236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -3575,8 +4334,14 @@
       <c r="L7">
         <v>0.10416555660000001</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>0.10228508059999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -3601,8 +4366,14 @@
       <c r="L8">
         <v>0.1061364964</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M8">
+        <v>0.1017539382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -3627,8 +4398,14 @@
       <c r="L9">
         <v>0.1713480808</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M9">
+        <v>0.10622836840000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -3653,8 +4430,14 @@
       <c r="L10">
         <v>0.17375513120000002</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M10">
+        <v>0.10837082360000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -3679,8 +4462,14 @@
       <c r="L11">
         <v>0.17614309440000001</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M11">
+        <v>0.1072073434</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -3705,8 +4494,14 @@
       <c r="L12">
         <v>0.30421219620000001</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M12">
+        <v>1.3223772467999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -3731,8 +4526,14 @@
       <c r="L13">
         <v>0.30963479440000002</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <v>1.3331471528000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -3757,8 +4558,14 @@
       <c r="L14">
         <v>0.30241801160000004</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M14">
+        <v>1.3240592006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -3783,8 +4590,14 @@
       <c r="L15">
         <v>0.90624064539999993</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M15">
+        <v>1.4603826568</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -3809,8 +4622,14 @@
       <c r="L16">
         <v>0.87383658139999998</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M16">
+        <v>1.4552879336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -3835,8 +4654,14 @@
       <c r="L17">
         <v>0.90894442400000008</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M17">
+        <v>1.5086068051999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -3861,8 +4686,14 @@
       <c r="L18">
         <v>2.3321801820000001</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M18">
+        <v>2.5140791085999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -3887,8 +4718,14 @@
       <c r="L19">
         <v>2.2653292417999999</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <v>2.4378431608</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -3913,8 +4750,14 @@
       <c r="L20">
         <v>2.3354903658000001</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M20">
+        <v>2.4468871848</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
@@ -3939,8 +4782,14 @@
       <c r="L21">
         <v>0.514506923</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M21">
+        <v>2.6050473487999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -3965,8 +4814,14 @@
       <c r="L22">
         <v>0.52251623160000005</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M22">
+        <v>2.5755155485999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -3991,8 +4846,14 @@
       <c r="L23">
         <v>0.51922512459999992</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M23">
+        <v>2.6116464557999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -4017,8 +4878,14 @@
       <c r="L24">
         <v>2.8231402779999999</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M24">
+        <v>4.056727167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -4043,8 +4910,14 @@
       <c r="L25">
         <v>2.7459344899999998</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M25">
+        <v>4.0729798146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
@@ -4060,8 +4933,14 @@
       <c r="L26">
         <v>3.0395307211999998</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M26">
+        <v>4.0742190645999994</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -4077,8 +4956,14 @@
       <c r="L27">
         <v>5.9594664666000003</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M27">
+        <v>7.0546997665999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -4094,8 +4979,14 @@
       <c r="L28">
         <v>6.1437438804000006</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M28">
+        <v>6.8088274506000008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -4111,8 +5002,14 @@
       <c r="L29">
         <v>5.9016621336000004</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M29">
+        <v>6.7390644667999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -4137,8 +5034,14 @@
       <c r="L31">
         <v>4.8561519800000001E-2</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M31">
+        <v>0.10440039320000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -4163,8 +5066,14 @@
       <c r="L32">
         <v>4.7091354600000003E-2</v>
       </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M32">
+        <v>0.1038452862</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -4189,8 +5098,14 @@
       <c r="L33">
         <v>4.74817352E-2</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M33">
+        <v>0.10391662040000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -4215,8 +5130,14 @@
       <c r="L34">
         <v>0.1110548616</v>
       </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M34">
+        <v>0.10629454320000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -4241,8 +5162,14 @@
       <c r="L35">
         <v>0.1122875012</v>
       </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M35">
+        <v>0.1075255276</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -4267,8 +5194,14 @@
       <c r="L36">
         <v>0.11700834959999999</v>
       </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M36">
+        <v>0.1073332204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -4293,8 +5226,14 @@
       <c r="L37">
         <v>0.21172243800000001</v>
       </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M37">
+        <v>0.11075707999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -4319,8 +5258,14 @@
       <c r="L38">
         <v>0.20632119319999997</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M38">
+        <v>0.11409548059999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -4345,8 +5290,14 @@
       <c r="L39">
         <v>0.20594084679999999</v>
       </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M39">
+        <v>0.11099471060000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -4371,8 +5322,14 @@
       <c r="L40">
         <v>0.28383177739999998</v>
       </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M40">
+        <v>1.3133093603999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -4397,8 +5354,14 @@
       <c r="L41">
         <v>0.30017881639999999</v>
       </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M41">
+        <v>1.321611404</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
@@ -4423,8 +5386,14 @@
       <c r="L42">
         <v>0.29862384199999997</v>
       </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M42">
+        <v>1.3237643213999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
@@ -4449,8 +5418,14 @@
       <c r="L43">
         <v>0.88542769479999994</v>
       </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M43">
+        <v>1.468181145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
@@ -4475,8 +5450,14 @@
       <c r="L44">
         <v>0.8643535443999999</v>
       </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M44">
+        <v>1.4699011103999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
       <c r="B45" t="s">
         <v>44</v>
       </c>
@@ -4501,8 +5482,14 @@
       <c r="L45">
         <v>0.88338929560000001</v>
       </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M45">
+        <v>1.475360486</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
@@ -4527,8 +5514,14 @@
       <c r="L46">
         <v>2.4278497884000001</v>
       </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M46">
+        <v>2.5461721341999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
@@ -4553,8 +5546,14 @@
       <c r="L47">
         <v>2.4924288818</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M47">
+        <v>2.5799957820000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
@@ -4579,8 +5578,14 @@
       <c r="L48">
         <v>2.4706621132</v>
       </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M48">
+        <v>2.5716838287999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
@@ -4605,8 +5610,14 @@
       <c r="L49">
         <v>0.48600756459999994</v>
       </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M49">
+        <v>2.5788498136000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
@@ -4631,8 +5642,14 @@
       <c r="L50">
         <v>0.48603566919999996</v>
       </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M50">
+        <v>2.5887278841999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
@@ -4657,8 +5674,14 @@
       <c r="L51">
         <v>0.49354915220000006</v>
       </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M51">
+        <v>2.5905841837999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
@@ -4683,8 +5706,14 @@
       <c r="L52">
         <v>2.7089298869999996</v>
       </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M52">
+        <v>4.1843065714000005</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
@@ -4709,8 +5738,14 @@
       <c r="L53">
         <v>2.7075117642000004</v>
       </c>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M53">
+        <v>4.0944368176000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
       <c r="B54" t="s">
         <v>53</v>
       </c>
@@ -4726,8 +5761,14 @@
       <c r="L54">
         <v>2.7917107078000005</v>
       </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M54">
+        <v>4.1685894755999993</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
       <c r="B55" t="s">
         <v>54</v>
       </c>
@@ -4743,8 +5784,14 @@
       <c r="L55">
         <v>6.0644811683999995</v>
       </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M55">
+        <v>6.6947047072000005</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
       <c r="B56" t="s">
         <v>55</v>
       </c>
@@ -4760,8 +5807,14 @@
       <c r="L56">
         <v>6.1032093060000001</v>
       </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M56">
+        <v>6.8179691652000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>70</v>
+      </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
@@ -4776,6 +5829,9 @@
       </c>
       <c r="L57">
         <v>6.0665173848</v>
+      </c>
+      <c r="M57">
+        <v>6.7481392364000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sim A, B, C, D, E all complete and results in csv
</commit_message>
<xml_diff>
--- a/Data/Scenarios/Graph List and Stats.xlsx
+++ b/Data/Scenarios/Graph List and Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marto\git\Algos_Assignment1\Data\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA1CCE2-0DFB-41C7-8752-ED279A477E16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41D6C5D-CFB8-413D-B3CC-E46D094B2E47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="48" windowWidth="21252" windowHeight="13608" activeTab="1" xr2:uid="{61CBB812-40D1-44A3-AFF3-2B0F76CA3C04}"/>
+    <workbookView xWindow="11412" yWindow="192" windowWidth="21252" windowHeight="13608" activeTab="1" xr2:uid="{61CBB812-40D1-44A3-AFF3-2B0F76CA3C04}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="4" r:id="rId1"/>
@@ -2184,7 +2184,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D71CDE3-7DBD-462C-93FC-85AE65D9340E}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2229,7 +2228,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>71</v>
       </c>
@@ -2267,7 +2266,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -2305,7 +2304,7 @@
         <v>3.9307000000000003E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -2343,7 +2342,7 @@
         <v>4.0774620000000002E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>4.2040706666666663E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -2465,7 +2464,7 @@
         <v>6.6559300000000013E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -2503,7 +2502,7 @@
         <v>6.1092039999999996E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -2587,7 +2586,7 @@
         <v>6.3448180000000005E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -2625,7 +2624,7 @@
         <v>7.0269000000000006E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -2663,7 +2662,7 @@
         <v>8.1755239999999996E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -2747,7 +2746,7 @@
         <v>7.6443086666666668E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -2785,7 +2784,7 @@
         <v>7.5599260000000002E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -2823,7 +2822,7 @@
         <v>9.5610539999999998E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -2907,7 +2906,7 @@
         <v>8.0199793333333329E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -2945,7 +2944,7 @@
         <v>8.5363859999999998E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -2983,7 +2982,7 @@
         <v>9.4207980000000013E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -3067,7 +3066,7 @@
         <v>8.6653066666666676E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -3102,7 +3101,7 @@
         <v>1.1726073999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -3137,7 +3136,7 @@
         <v>8.8568999999999996E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -3214,7 +3213,7 @@
         <v>9.647733333333332E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -3249,7 +3248,7 @@
         <v>8.9449180000000014E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -3284,7 +3283,7 @@
         <v>6.698867999999998E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -3361,7 +3360,7 @@
         <v>7.89572E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -3396,7 +3395,7 @@
         <v>7.9549999999999998E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -3431,7 +3430,7 @@
         <v>8.6468060000000004E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -3499,7 +3498,7 @@
         <v>8.3594879999999993E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -3525,7 +3524,7 @@
         <v>9.9192820000000006E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -3551,7 +3550,7 @@
         <v>9.5785300000000005E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -3619,7 +3618,7 @@
         <v>1.0240387333333332E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -3657,7 +3656,7 @@
         <v>2.9433200000000001E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -3695,7 +3694,7 @@
         <v>2.3583980000000003E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -3779,7 +3778,7 @@
         <v>2.589124E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -3817,7 +3816,7 @@
         <v>3.8812359999999997E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -3855,7 +3854,7 @@
         <v>3.7515280000000002E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -3939,7 +3938,7 @@
         <v>3.809420666666666E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -3977,7 +3976,7 @@
         <v>5.2599539999999994E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -4015,7 +4014,7 @@
         <v>4.6431359999999999E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -4099,7 +4098,7 @@
         <v>4.7385006666666665E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>70</v>
       </c>
@@ -4137,7 +4136,7 @@
         <v>5.0745E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>70</v>
       </c>
@@ -4175,7 +4174,7 @@
         <v>2.8597080000000003E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -4259,7 +4258,7 @@
         <v>3.7369993333333332E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -4297,7 +4296,7 @@
         <v>9.0808360000000005E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -4335,7 +4334,7 @@
         <v>5.4991940000000009E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -4419,7 +4418,7 @@
         <v>6.6658486666666683E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -4454,7 +4453,7 @@
         <v>7.3695480000000001E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -4489,7 +4488,7 @@
         <v>6.6003320000000004E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -4566,7 +4565,7 @@
         <v>7.0227120000000004E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -4601,7 +4600,7 @@
         <v>2.9944059999999998E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -4636,7 +4635,7 @@
         <v>2.5998079999999999E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -4713,7 +4712,7 @@
         <v>2.6988339999999998E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -4748,7 +4747,7 @@
         <v>3.9991020000000003E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -4783,7 +4782,7 @@
         <v>4.2825759999999996E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -4851,7 +4850,7 @@
         <v>4.1227046666666664E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -4877,7 +4876,7 @@
         <v>5.6602159999999987E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -4903,7 +4902,7 @@
         <v>5.1168840000000008E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -4972,13 +4971,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N74" xr:uid="{8428BEEC-3A27-45C6-A9DA-4A78069BC47A}">
-    <filterColumn colId="4">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N74" xr:uid="{8428BEEC-3A27-45C6-A9DA-4A78069BC47A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>